<commit_message>
Add affiliations to Investigation persons
</commit_message>
<xml_diff>
--- a/isa.investigation.xlsx
+++ b/isa.investigation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\invenio-test-arc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\invenio-test-arc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0C998F-48A5-4F27-94CF-692DB1F38030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9B6EFA-C449-4210-AEF8-1A5C3DBC591B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_investigation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="109">
   <si>
     <t>ONTOLOGY SOURCE REFERENCE</t>
   </si>
@@ -348,6 +348,18 @@
   </si>
   <si>
     <t>testuser@nfdi4plants.org</t>
+  </si>
+  <si>
+    <t>RPTU</t>
+  </si>
+  <si>
+    <t>ALUF</t>
+  </si>
+  <si>
+    <t>TestUni</t>
+  </si>
+  <si>
+    <t>TestHS</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1214,7 @@
   <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,16 +1464,16 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add ORCIDs for every test person
Closes #2.
</commit_message>
<xml_diff>
--- a/isa.investigation.xlsx
+++ b/isa.investigation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\invenio-test-arc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9B6EFA-C449-4210-AEF8-1A5C3DBC591B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116FBBEE-6894-4878-9BF2-C4B595076C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_investigation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="114">
   <si>
     <t>ONTOLOGY SOURCE REFERENCE</t>
   </si>
@@ -140,6 +140,15 @@
     <t>Investigation Person Email</t>
   </si>
   <si>
+    <t>weil@nfdi4plants.org</t>
+  </si>
+  <si>
+    <t>tschoepe@nfdi4plants.org</t>
+  </si>
+  <si>
+    <t>testuser@nfdi4plants.org</t>
+  </si>
+  <si>
     <t>Investigation Person Phone</t>
   </si>
   <si>
@@ -152,6 +161,18 @@
     <t>Investigation Person Affiliation</t>
   </si>
   <si>
+    <t>RPTU</t>
+  </si>
+  <si>
+    <t>ALUF</t>
+  </si>
+  <si>
+    <t>TestUni</t>
+  </si>
+  <si>
+    <t>TestHS</t>
+  </si>
+  <si>
     <t>Investigation Person Roles</t>
   </si>
   <si>
@@ -161,6 +182,12 @@
     <t>Investigation Person Roles Term Source REF</t>
   </si>
   <si>
+    <t>Comment[&lt;Investigation Person ORCID&gt;]</t>
+  </si>
+  <si>
+    <t>orcid1</t>
+  </si>
+  <si>
     <t>STUDY</t>
   </si>
   <si>
@@ -341,25 +368,13 @@
     <t>Study Person Roles Term Source REF</t>
   </si>
   <si>
-    <t>weil@nfdi4plants.org</t>
-  </si>
-  <si>
-    <t>tschoepe@nfdi4plants.org</t>
-  </si>
-  <si>
-    <t>testuser@nfdi4plants.org</t>
-  </si>
-  <si>
-    <t>RPTU</t>
-  </si>
-  <si>
-    <t>ALUF</t>
-  </si>
-  <si>
-    <t>TestUni</t>
-  </si>
-  <si>
-    <t>TestHS</t>
+    <t>orcid2</t>
+  </si>
+  <si>
+    <t>orcid3</t>
+  </si>
+  <si>
+    <t>orcid4</t>
   </si>
 </sst>
 </file>
@@ -502,9 +517,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -807,7 +820,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -850,13 +863,11 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -887,7 +898,6 @@
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Link" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
@@ -1211,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,22 +1405,22 @@
       <c r="A24" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>104</v>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -1427,7 +1437,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -1444,7 +1454,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -1461,24 +1471,24 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>108</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -1495,7 +1505,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -1512,7 +1522,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -1529,20 +1539,29 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -1550,7 +1569,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -1558,7 +1577,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -1566,7 +1585,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -1574,7 +1593,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -1582,276 +1601,279 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>57</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>101</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B24" r:id="rId1" xr:uid="{CA6EEBE9-B031-4311-837C-20312E6F8637}"/>
-    <hyperlink ref="C24" r:id="rId2" xr:uid="{AF6EE784-5F25-42B0-A338-CCEA01813FEA}"/>
-    <hyperlink ref="D24" r:id="rId3" xr:uid="{7C55E1F7-EC51-400A-A1EB-12E076E601C0}"/>
-    <hyperlink ref="E24" r:id="rId4" xr:uid="{EBF10B08-DDC5-499A-8DB0-EEE6F17CA19A}"/>
-  </hyperlinks>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update ORCID for ORCID number scheme
</commit_message>
<xml_diff>
--- a/isa.investigation.xlsx
+++ b/isa.investigation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schne\source\repos\nfdi4plants\invenio-test-arc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\invenio-test-arc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C49C1D-B955-43BC-8281-97FA980C1C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AC1218-2E2D-4DEA-BF2B-114343A16367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43380" yWindow="3330" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_investigation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="115">
   <si>
     <t>ONTOLOGY SOURCE REFERENCE</t>
   </si>
@@ -185,9 +185,6 @@
     <t>Comment[&lt;Investigation Person ORCID&gt;]</t>
   </si>
   <si>
-    <t>orcid1</t>
-  </si>
-  <si>
     <t>STUDY</t>
   </si>
   <si>
@@ -368,16 +365,19 @@
     <t>Study Person Roles Term Source REF</t>
   </si>
   <si>
-    <t>orcid2</t>
-  </si>
-  <si>
-    <t>orcid3</t>
-  </si>
-  <si>
-    <t>orcid4</t>
-  </si>
-  <si>
     <t>Investigation description here please</t>
+  </si>
+  <si>
+    <t>1234-5678-9101-1121</t>
+  </si>
+  <si>
+    <t>0123-4567-8910-1112</t>
+  </si>
+  <si>
+    <t>0000-1111-2222-3333</t>
+  </si>
+  <si>
+    <t>0123-1234-2345-3456</t>
   </si>
 </sst>
 </file>
@@ -871,48 +871,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -928,7 +928,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1227,10 +1227,10 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
@@ -1289,7 +1289,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1545,26 +1545,26 @@
         <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D32" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E32" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -1612,267 +1612,267 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replace made-up ORCIDs with functioning ones
</commit_message>
<xml_diff>
--- a/isa.investigation.xlsx
+++ b/isa.investigation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\invenio-test-arc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AC1218-2E2D-4DEA-BF2B-114343A16367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B023ED2-EDB9-4A3A-ADEA-0ED07434007F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_investigation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="112">
   <si>
     <t>ONTOLOGY SOURCE REFERENCE</t>
   </si>
@@ -368,16 +368,7 @@
     <t>Investigation description here please</t>
   </si>
   <si>
-    <t>1234-5678-9101-1121</t>
-  </si>
-  <si>
-    <t>0123-4567-8910-1112</t>
-  </si>
-  <si>
-    <t>0000-1111-2222-3333</t>
-  </si>
-  <si>
-    <t>0123-1234-2345-3456</t>
+    <t>0000-0001-5874-2232</t>
   </si>
 </sst>
 </file>
@@ -1548,13 +1539,13 @@
         <v>111</v>
       </c>
       <c r="C32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E32" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>